<commit_message>
Commit live con gli studenti
aggiunti file a caso
</commit_message>
<xml_diff>
--- a/Seminario Catania/Orari seminario.xlsx
+++ b/Seminario Catania/Orari seminario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="16">
   <si>
     <t>Data</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Introduzione QuantLib</t>
+  </si>
+  <si>
+    <t>Git</t>
   </si>
 </sst>
 </file>
@@ -541,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -740,7 +743,9 @@
       <c r="G15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="I15" s="12" t="s">
         <v>11</v>
       </c>
@@ -760,7 +765,9 @@
       <c r="G16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="11"/>
+      <c r="H16" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="12" t="s">
         <v>11</v>
       </c>
@@ -780,7 +787,9 @@
       <c r="G17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="I17" s="12" t="s">
         <v>11</v>
       </c>
@@ -800,7 +809,9 @@
       <c r="G18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="11"/>
+      <c r="H18" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="I18" s="12" t="s">
         <v>11</v>
       </c>
@@ -815,12 +826,14 @@
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="H19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="11"/>
       <c r="I19" s="12" t="s">
         <v>11</v>
       </c>
@@ -831,16 +844,18 @@
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="H20" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="11"/>
       <c r="I20" s="12" t="s">
         <v>11</v>
       </c>
@@ -962,7 +977,7 @@
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -978,7 +993,7 @@
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>

</xml_diff>